<commit_message>
include new files from Emmas last day at the lab
</commit_message>
<xml_diff>
--- a/data/raw_data/depths.xlsx
+++ b/data/raw_data/depths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/denali_ecm-to_emma/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Desktop/UW/ECM/denali_ECM/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9C1343-DF91-D047-B4CA-23BB2A907C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079383C8-BCC0-204D-B9A9-FD199FBC7A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="760" windowWidth="29240" windowHeight="18880" xr2:uid="{BD19F855-352E-A240-B61F-DA1958A1D0A0}"/>
+    <workbookView xWindow="1000" yWindow="880" windowWidth="17320" windowHeight="18760" xr2:uid="{BD19F855-352E-A240-B61F-DA1958A1D0A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="10">
   <si>
     <t>core</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>dic1</t>
+  </si>
+  <si>
+    <t>184a</t>
+  </si>
+  <si>
+    <t>188a</t>
+  </si>
+  <si>
+    <t>188b</t>
+  </si>
+  <si>
+    <t>187a</t>
+  </si>
+  <si>
+    <t>187b</t>
   </si>
 </sst>
 </file>
@@ -445,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6114CE1F-2BF5-A349-A50F-6D82EE1E16D1}">
   <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1500,6 +1515,76 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0.1</v>
+      </c>
+    </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1565,6 +1650,9 @@
       <c r="C130" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D131">
+    <sortCondition ref="B1:B131"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>